<commit_message>
Partially implemented config menu design.
</commit_message>
<xml_diff>
--- a/Documentation/Documentation Logbook.xlsx
+++ b/Documentation/Documentation Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7B931C-79DC-4519-8D34-F8C9CFBEE5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A019AA-AF1C-4AB2-8549-434D025ECAFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Started documentation and design.</t>
+  </si>
+  <si>
+    <t>Chose colour pallette and designed config page</t>
+  </si>
+  <si>
+    <t>Designed colour pallette and config page. Partially implemented config page. Also began designing various symbols for use as mode selection.</t>
   </si>
 </sst>
 </file>
@@ -103,15 +109,6 @@
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -124,10 +121,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -446,7 +452,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:G11"/>
+      <selection activeCell="E13" sqref="E13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -457,32 +463,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1"/>
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -492,295 +498,279 @@
       <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="2">
         <v>44133</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="6"/>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44134</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="1"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="1"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="1"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.35">
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
     <mergeCell ref="A1:A30"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -791,6 +781,30 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="E12:G12"/>
     <mergeCell ref="E13:G13"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the base for movement, and enabled visible player
</commit_message>
<xml_diff>
--- a/Documentation/Documentation Logbook.xlsx
+++ b/Documentation/Documentation Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A019AA-AF1C-4AB2-8549-434D025ECAFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12283FB2-B6A7-47B1-8CBA-7BAB9B7F9452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -64,6 +64,27 @@
   </si>
   <si>
     <t>Designed colour pallette and config page. Partially implemented config page. Also began designing various symbols for use as mode selection.</t>
+  </si>
+  <si>
+    <t>Completed controls between menus and added a title for the config page. Also created a gantt chart.</t>
+  </si>
+  <si>
+    <t>Continued creating Gantt chart</t>
+  </si>
+  <si>
+    <t>Added more parts and features to the gannt chart.</t>
+  </si>
+  <si>
+    <t>As title.</t>
+  </si>
+  <si>
+    <t>Began designing auto map loading.</t>
+  </si>
+  <si>
+    <t>Brainstormed with ideas about map generation. Wrote stub functions for most processes involved in map generation.</t>
+  </si>
+  <si>
+    <t>Added a basic sprite.</t>
   </si>
 </sst>
 </file>
@@ -106,34 +127,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -452,322 +467,353 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:G13"/>
+      <selection activeCell="E25" sqref="E25:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.08984375" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" customWidth="1"/>
-    <col min="4" max="7" width="30.6328125" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="7"/>
+    <col min="2" max="2" width="9.08984375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" style="7" customWidth="1"/>
+    <col min="4" max="7" width="30.6328125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="6"/>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.5">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="4"/>
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="1">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="4"/>
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>44133</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
-      <c r="B6" s="1">
+      <c r="A6" s="4"/>
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>44134</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+      <c r="A7" s="4"/>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44153</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44154</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4"/>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44166</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4"/>
+      <c r="B10" s="2">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43836</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="6"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.35">
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="34">

</xml_diff>

<commit_message>
Version 2 for 18/01/2021
</commit_message>
<xml_diff>
--- a/Documentation/Documentation Logbook.xlsx
+++ b/Documentation/Documentation Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12283FB2-B6A7-47B1-8CBA-7BAB9B7F9452}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3CD44E-805D-449D-97CF-ED98DB4587B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Added a basic sprite.</t>
+  </si>
+  <si>
+    <t>Just a rectangle to begin with.</t>
+  </si>
+  <si>
+    <t>Fixed bug, began implementing player movement</t>
+  </si>
+  <si>
+    <t>Rectangle didn't display upon loading. Fixed this error and implemented player movement using the WASD keys.</t>
   </si>
 </sst>
 </file>
@@ -136,7 +145,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -148,7 +157,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,15 +476,15 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:G25"/>
+      <selection activeCell="E11" sqref="E11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="7"/>
-    <col min="2" max="2" width="9.08984375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="10.90625" style="7" customWidth="1"/>
-    <col min="4" max="7" width="30.6328125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="9.08984375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" style="3" customWidth="1"/>
+    <col min="4" max="7" width="30.6328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.5">
@@ -505,13 +514,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
@@ -531,11 +540,11 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
@@ -548,11 +557,11 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
@@ -565,11 +574,11 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
@@ -582,11 +591,11 @@
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
@@ -599,11 +608,11 @@
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
@@ -611,194 +620,204 @@
         <v>6</v>
       </c>
       <c r="C10" s="1">
-        <v>43836</v>
+        <v>44202</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>44214</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E31" s="4"/>
@@ -817,6 +836,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
     <mergeCell ref="A1:A30"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -833,24 +870,6 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E23:G23"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed borders not moving. Border class now works as intended, just doesn't display sprites. Will create new sprite and add that to the game.
</commit_message>
<xml_diff>
--- a/Documentation/Documentation Logbook.xlsx
+++ b/Documentation/Documentation Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3CD44E-805D-449D-97CF-ED98DB4587B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC024E9-52D3-4E32-89E7-A55ADE52DE30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Rectangle didn't display upon loading. Fixed this error and implemented player movement using the WASD keys.</t>
+  </si>
+  <si>
+    <t>Finished implementing player movement. Began implementing border generation and movement.</t>
+  </si>
+  <si>
+    <t>Fixed player movement bug where the character wouldn’t always move in the desired direction. Began to implement Border() class and attempted to make them visible.</t>
   </si>
 </sst>
 </file>
@@ -476,7 +482,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:G11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -648,18 +654,28 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>44220</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <v>9</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
       <c r="E13" s="7"/>

</xml_diff>

<commit_message>
Made movement.Began adding other borders and fixing placement.
</commit_message>
<xml_diff>
--- a/Documentation/Documentation Logbook.xlsx
+++ b/Documentation/Documentation Logbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abram\Documents\IT\Major Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC024E9-52D3-4E32-89E7-A55ADE52DE30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00597F3-0676-4BBA-9945-74F91073EC4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{A4DA64FF-B9B3-4233-BC20-5B0DAEA49FF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Abram Liddell</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Fixed player movement bug where the character wouldn’t always move in the desired direction. Began to implement Border() class and attempted to make them visible.</t>
+  </si>
+  <si>
+    <t>Finished border generation and movement. Began finalised sprites.</t>
+  </si>
+  <si>
+    <t>Border generation and movement now working as intended. There is a bug with the borders not displaying, but that will be fixed later.</t>
   </si>
 </sst>
 </file>
@@ -154,16 +160,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -482,7 +488,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E13" sqref="E13:G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -494,8 +500,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.5">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C1" s="6"/>
@@ -503,7 +509,7 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -512,14 +518,14 @@
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
@@ -536,7 +542,7 @@
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -546,14 +552,14 @@
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2">
         <v>2</v>
       </c>
@@ -563,14 +569,14 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="58" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2">
         <v>3</v>
       </c>
@@ -580,14 +586,14 @@
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="2">
         <v>4</v>
       </c>
@@ -597,14 +603,14 @@
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="2">
         <v>5</v>
       </c>
@@ -614,14 +620,14 @@
       <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="2">
         <v>6</v>
       </c>
@@ -631,14 +637,14 @@
       <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="B11" s="2">
         <v>7</v>
       </c>
@@ -648,14 +654,14 @@
       <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2">
         <v>8</v>
       </c>
@@ -665,211 +671,199 @@
       <c r="D12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="5"/>
       <c r="B13" s="2">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="C13" s="1">
+        <v>44250</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
+      <c r="A24" s="5"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
+      <c r="A25" s="5"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
+      <c r="A26" s="5"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
+      <c r="A30" s="5"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.35">
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="E19:G19"/>
     <mergeCell ref="A1:A30"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -886,6 +880,24 @@
     <mergeCell ref="E21:G21"/>
     <mergeCell ref="E22:G22"/>
     <mergeCell ref="E23:G23"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="E33:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>